<commit_message>
added new variable in clearance function in blanks.py.
added two new functions (`contain` and `semicolon_list`) in general.py
</commit_message>
<xml_diff>
--- a/files/File Input.xlsx
+++ b/files/File Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20375"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Laporan Kunjungan Kapal\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal Programming\Laporan Kunjungan Kapal\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C5BEF0-0820-481C-87E3-C6EC544020FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425507AF-78F0-4166-BACC-5C25685D7906}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rekap Bunyu" sheetId="1" r:id="rId1"/>
@@ -19,24 +19,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Rekap Bunyu'!$A$1:$AK$289</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8451" uniqueCount="1256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8449" uniqueCount="1256">
   <si>
     <t>NO</t>
   </si>
@@ -4881,9 +4869,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK345"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2:L345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -4944,7 +4932,7 @@
       <c r="G1" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="54" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="54" t="s">
@@ -21436,8 +21424,8 @@
       <c r="K143" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="L143" s="70" t="s">
-        <v>122</v>
+      <c r="L143" s="70">
+        <v>0</v>
       </c>
       <c r="M143" s="13" t="s">
         <v>177</v>
@@ -45066,8 +45054,8 @@
       <c r="K345" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="L345" s="9" t="s">
-        <v>473</v>
+      <c r="L345" s="9">
+        <v>0</v>
       </c>
       <c r="M345" s="3" t="s">
         <v>177</v>

</xml_diff>